<commit_message>
Worked on SFD model, forces need work
</commit_message>
<xml_diff>
--- a/SFD/sfd_inputs.xlsx
+++ b/SFD/sfd_inputs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garyh\OneDrive\Desktop\Purdue\PSP\Pathfinder\PSPL_Rocket_A\SFD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83F9B47-4560-49AF-8D38-71504627931B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4ED30D-A3EF-4A9F-AED3-216D118269DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle Sections" sheetId="1" r:id="rId1"/>
-    <sheet name="Point Masses" sheetId="2" r:id="rId2"/>
+    <sheet name="Aerodynamic Properties" sheetId="3" r:id="rId2"/>
+    <sheet name="Point Masses" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -107,6 +108,36 @@
   </si>
   <si>
     <t>Batteries</t>
+  </si>
+  <si>
+    <t>Off the rail</t>
+  </si>
+  <si>
+    <t>Max Q</t>
+  </si>
+  <si>
+    <t>Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Acceleration (m/s^2)</t>
+  </si>
+  <si>
+    <t>Mach</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>Thrust (lbf)</t>
+  </si>
+  <si>
+    <t>Max wind gust (mph)</t>
+  </si>
+  <si>
+    <t>AoA</t>
+  </si>
+  <si>
+    <t>Air Density</t>
   </si>
 </sst>
 </file>
@@ -426,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,6 +669,30 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -645,6 +700,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF315E06-1D24-4B8B-B483-A56CF72D8637}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>29.7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60611FD-C62F-4AF0-80C9-010A552DCB1C}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added inertia, tested existing code, still need to add forces code and drag
</commit_message>
<xml_diff>
--- a/SFD/sfd_inputs.xlsx
+++ b/SFD/sfd_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garyh\OneDrive\Desktop\Purdue\PSP\Pathfinder\PSPL_Rocket_A\SFD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4ED30D-A3EF-4A9F-AED3-216D118269DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38C9D9E-C13C-44C3-84C7-24F89E1E8026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -814,7 +814,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,10 +839,10 @@
         <v>26</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checked shear and bending code, need to add values for them
</commit_message>
<xml_diff>
--- a/SFD/sfd_inputs.xlsx
+++ b/SFD/sfd_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garyh\OneDrive\Desktop\Purdue\PSP\Pathfinder\PSPL_Rocket_A\SFD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85584A4-4038-442A-AAA4-93E6B3A39BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA69A7D-7440-47EA-928E-F4473A56E228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle Sections" sheetId="1" r:id="rId1"/>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,10 +582,10 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4.42</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF315E06-1D24-4B8B-B483-A56CF72D8637}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished shear and bending code? still need proper inputs
</commit_message>
<xml_diff>
--- a/SFD/sfd_inputs.xlsx
+++ b/SFD/sfd_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garyh\OneDrive\Desktop\Purdue\PSP\Pathfinder\PSPL_Rocket_A\SFD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA69A7D-7440-47EA-928E-F4473A56E228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A3D1C1-1568-4D11-BB45-968EB0ABD6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,21 @@
     <sheet name="Aerodynamic Properties" sheetId="3" r:id="rId2"/>
     <sheet name="Point Masses" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -458,7 +469,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -543,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -557,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -571,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -582,10 +593,11 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>4.42</v>
+        <v>4.4242043000000004</v>
       </c>
       <c r="C6">
-        <v>8.8000000000000007</v>
+        <f>4.5737205 / 12</f>
+        <v>0.38114337500000001</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -605,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.23774000000000001</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -616,10 +628,11 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>4.4242043000000004</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <f>4.5737205 / 12</f>
+        <v>0.38114337500000001</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -639,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -653,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -704,7 +717,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added comments for sfd, put in available proper inputs, final tasks are axial function, proper inputs, and validation
</commit_message>
<xml_diff>
--- a/SFD/sfd_inputs.xlsx
+++ b/SFD/sfd_inputs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garyh\OneDrive\Desktop\Purdue\PSP\Pathfinder\PSPL_Rocket_A\SFD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0eae142ebbf7e355/Desktop/Purdue/PSP/Pathfinder/PSPL_Rocket_A/SFD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A3D1C1-1568-4D11-BB45-968EB0ABD6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D4A3D1C1-1568-4D11-BB45-968EB0ABD6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC1C4F36-CF35-48D1-833B-AFF298C5FE96}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,6 +201,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,7 +473,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -717,7 +721,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,10 +771,12 @@
         <v>29.7</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <f>6.8*9.81</f>
+        <v>66.707999999999998</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <f>29.7/343</f>
+        <v>8.6588921282798825E-2</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -793,13 +799,15 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <f>0.45*343</f>
+        <v>154.35</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <f>7.47*9.81</f>
+        <v>73.280699999999996</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.45</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>

<commit_message>
commented out angular acceleration from shear force calc
</commit_message>
<xml_diff>
--- a/SFD/sfd_inputs.xlsx
+++ b/SFD/sfd_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0eae142ebbf7e355/Desktop/Purdue/PSP/Pathfinder/PSPL_Rocket_A/SFD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D4A3D1C1-1568-4D11-BB45-968EB0ABD6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC1C4F36-CF35-48D1-833B-AFF298C5FE96}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{D4A3D1C1-1568-4D11-BB45-968EB0ABD6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C103ADF-0771-46C4-8EF1-70CFF4118B3A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,14 +600,14 @@
         <v>4.4242043000000004</v>
       </c>
       <c r="C6">
-        <f>4.5737205 / 12</f>
-        <v>0.38114337500000001</v>
+        <f>4.6/12</f>
+        <v>0.3833333333333333</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>4.42</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -635,14 +635,14 @@
         <v>4.4242043000000004</v>
       </c>
       <c r="C8">
-        <f>4.5737205 / 12</f>
-        <v>0.38114337500000001</v>
+        <f>6 / 12</f>
+        <v>0.5</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>4.42</v>
       </c>
       <c r="F8">
         <v>3</v>

</xml_diff>

<commit_message>
wrote on excel file
</commit_message>
<xml_diff>
--- a/SFD/sfd_inputs.xlsx
+++ b/SFD/sfd_inputs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0eae142ebbf7e355/Desktop/Purdue/PSP/Pathfinder/PSPL_Rocket_A/SFD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garyh\OneDrive\Desktop\Purdue\PSP\Pathfinder\PSPL_Rocket_A\SFD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{D4A3D1C1-1568-4D11-BB45-968EB0ABD6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C103ADF-0771-46C4-8EF1-70CFF4118B3A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C028288-1252-4208-A204-DB3242DA435B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,10 +201,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>